<commit_message>
add l/r_monomer_alphabet to xlink xlsx and yml
</commit_message>
<xml_diff>
--- a/bcforms/xlink/xlink_simple.xlsx
+++ b/bcforms/xlink/xlink_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoyuezheng/Desktop/karrlab/projects/bcforms/bcforms/xlink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041A553B-48A3-624C-8B45-F9FAC5BD9797}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C59D36-AE49-6246-B6B4-C5A4C5417573}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16200" xr2:uid="{091FBCF7-AB49-3546-8B60-F04EB334A316}"/>
+    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="16200" xr2:uid="{091FBCF7-AB49-3546-8B60-F04EB334A316}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="238">
   <si>
     <t>index</t>
   </si>
@@ -736,6 +736,15 @@
   </si>
   <si>
     <t>glycyl_lysine_isopeptide</t>
+  </si>
+  <si>
+    <t>left_monomer_alphabet</t>
+  </si>
+  <si>
+    <t>bpforms.ProteinForm</t>
+  </si>
+  <si>
+    <t>right_monomer_alphabet</t>
   </si>
 </sst>
 </file>
@@ -1090,15 +1099,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D26CF6B-E6EE-114C-9D76-237F535B67EE}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,31 +1139,37 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1171,31 +1186,37 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
+        <v>236</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1215,31 +1236,37 @@
         <v>31</v>
       </c>
       <c r="K3" t="s">
+        <v>236</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>26</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1262,31 +1289,37 @@
         <v>35</v>
       </c>
       <c r="K4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L4" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>38</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>39</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q4" t="s">
         <v>40</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>42</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1309,31 +1342,37 @@
         <v>47</v>
       </c>
       <c r="K5" t="s">
+        <v>236</v>
+      </c>
+      <c r="L5" t="s">
         <v>40</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>48</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>43</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q5" t="s">
         <v>24</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>26</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1356,31 +1395,37 @@
         <v>51</v>
       </c>
       <c r="K6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L6" t="s">
         <v>40</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>41</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>42</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>43</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q6" t="s">
         <v>52</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>54</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
@@ -1397,31 +1442,37 @@
         <v>58</v>
       </c>
       <c r="K7" t="s">
+        <v>236</v>
+      </c>
+      <c r="L7" t="s">
         <v>59</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>60</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>61</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>62</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q7" t="s">
         <v>59</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>64</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1444,31 +1495,37 @@
         <v>67</v>
       </c>
       <c r="K8" t="s">
+        <v>236</v>
+      </c>
+      <c r="L8" t="s">
         <v>20</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>68</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>69</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>23</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q8" t="s">
         <v>24</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>26</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1491,31 +1548,37 @@
         <v>72</v>
       </c>
       <c r="K9" t="s">
+        <v>236</v>
+      </c>
+      <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>27</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q9" t="s">
         <v>73</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>74</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>75</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17</v>
       </c>
@@ -1538,31 +1601,37 @@
         <v>79</v>
       </c>
       <c r="K10" t="s">
+        <v>236</v>
+      </c>
+      <c r="L10" t="s">
         <v>80</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>53</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>81</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>82</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q10" t="s">
         <v>24</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>25</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>26</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1585,31 +1654,37 @@
         <v>85</v>
       </c>
       <c r="K11" t="s">
+        <v>236</v>
+      </c>
+      <c r="L11" t="s">
         <v>86</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>37</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>87</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>88</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q11" t="s">
         <v>24</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>25</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>26</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19</v>
       </c>
@@ -1632,31 +1707,37 @@
         <v>91</v>
       </c>
       <c r="K12" t="s">
+        <v>236</v>
+      </c>
+      <c r="L12" t="s">
         <v>59</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>21</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>48</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>62</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q12" t="s">
         <v>24</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>25</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>26</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -1679,31 +1760,37 @@
         <v>94</v>
       </c>
       <c r="K13" t="s">
+        <v>236</v>
+      </c>
+      <c r="L13" t="s">
         <v>95</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>21</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>48</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>96</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q13" t="s">
         <v>24</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>25</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>26</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>24</v>
       </c>
@@ -1726,31 +1813,37 @@
         <v>100</v>
       </c>
       <c r="K14" t="s">
+        <v>236</v>
+      </c>
+      <c r="L14" t="s">
         <v>40</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>21</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>48</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q14" t="s">
         <v>101</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>102</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>103</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>25</v>
       </c>
@@ -1767,31 +1860,37 @@
         <v>107</v>
       </c>
       <c r="K15" t="s">
+        <v>236</v>
+      </c>
+      <c r="L15" t="s">
         <v>52</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>53</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>54</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>55</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q15" t="s">
         <v>108</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>109</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>110</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>29</v>
       </c>
@@ -1808,31 +1907,37 @@
         <v>114</v>
       </c>
       <c r="K16" t="s">
+        <v>236</v>
+      </c>
+      <c r="L16" t="s">
         <v>86</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>63</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>64</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>88</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q16" t="s">
         <v>115</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>21</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>116</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -1849,31 +1954,37 @@
         <v>120</v>
       </c>
       <c r="K17" t="s">
+        <v>236</v>
+      </c>
+      <c r="L17" t="s">
         <v>108</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>121</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>103</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>111</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q17" t="s">
         <v>108</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>122</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>123</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>37</v>
       </c>
@@ -1890,31 +2001,37 @@
         <v>125</v>
       </c>
       <c r="K18" t="s">
+        <v>236</v>
+      </c>
+      <c r="L18" t="s">
         <v>24</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>25</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>26</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>27</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q18" t="s">
         <v>36</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>122</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>126</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>44</v>
       </c>
@@ -1937,31 +2054,37 @@
         <v>128</v>
       </c>
       <c r="K19" t="s">
+        <v>236</v>
+      </c>
+      <c r="L19" t="s">
         <v>24</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>25</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>26</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>27</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q19" t="s">
         <v>129</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>53</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="S19" t="s">
         <v>81</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>45</v>
       </c>
@@ -1978,31 +2101,37 @@
         <v>132</v>
       </c>
       <c r="K20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L20" t="s">
         <v>24</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>25</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>26</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>27</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q20" t="s">
         <v>73</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>122</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
         <v>126</v>
       </c>
-      <c r="R20" t="s">
+      <c r="T20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>48</v>
       </c>
@@ -2025,31 +2154,37 @@
         <v>134</v>
       </c>
       <c r="K21" t="s">
+        <v>236</v>
+      </c>
+      <c r="L21" t="s">
         <v>24</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>25</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>26</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>27</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q21" t="s">
         <v>115</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>21</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="S21" t="s">
         <v>116</v>
       </c>
-      <c r="R21" t="s">
+      <c r="T21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -2066,31 +2201,37 @@
         <v>136</v>
       </c>
       <c r="K22" t="s">
+        <v>236</v>
+      </c>
+      <c r="L22" t="s">
         <v>24</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>25</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>26</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>27</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q22" t="s">
         <v>101</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>137</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="S22" t="s">
         <v>138</v>
       </c>
-      <c r="R22" t="s">
+      <c r="T22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>55</v>
       </c>
@@ -2107,31 +2248,37 @@
         <v>140</v>
       </c>
       <c r="K23" t="s">
+        <v>236</v>
+      </c>
+      <c r="L23" t="s">
         <v>24</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>25</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>26</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>27</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q23" t="s">
         <v>59</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>141</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="S23" t="s">
         <v>142</v>
       </c>
-      <c r="R23" t="s">
+      <c r="T23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>57</v>
       </c>
@@ -2148,31 +2295,37 @@
         <v>144</v>
       </c>
       <c r="K24" t="s">
+        <v>236</v>
+      </c>
+      <c r="L24" t="s">
         <v>36</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>21</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>22</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>39</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q24" t="s">
         <v>108</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>145</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="S24" t="s">
         <v>146</v>
       </c>
-      <c r="R24" t="s">
+      <c r="T24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>58</v>
       </c>
@@ -2195,31 +2348,37 @@
         <v>148</v>
       </c>
       <c r="K25" t="s">
+        <v>236</v>
+      </c>
+      <c r="L25" t="s">
         <v>36</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>37</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>38</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>39</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q25" t="s">
         <v>86</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>63</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="S25" t="s">
         <v>64</v>
       </c>
-      <c r="R25" t="s">
+      <c r="T25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>61</v>
       </c>
@@ -2242,31 +2401,37 @@
         <v>150</v>
       </c>
       <c r="K26" t="s">
+        <v>236</v>
+      </c>
+      <c r="L26" t="s">
         <v>52</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>53</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>54</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>55</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q26" t="s">
         <v>101</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>102</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="S26" t="s">
         <v>103</v>
       </c>
-      <c r="R26" t="s">
+      <c r="T26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>63</v>
       </c>
@@ -2289,31 +2454,37 @@
         <v>152</v>
       </c>
       <c r="K27" t="s">
+        <v>236</v>
+      </c>
+      <c r="L27" t="s">
         <v>80</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>53</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>81</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>82</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q27" t="s">
         <v>101</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>102</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="S27" t="s">
         <v>103</v>
       </c>
-      <c r="R27" t="s">
+      <c r="T27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>64</v>
       </c>
@@ -2330,31 +2501,37 @@
         <v>154</v>
       </c>
       <c r="K28" t="s">
+        <v>236</v>
+      </c>
+      <c r="L28" t="s">
         <v>80</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>155</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>156</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>82</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q28" t="s">
         <v>157</v>
       </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
         <v>74</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="S28" t="s">
         <v>26</v>
       </c>
-      <c r="R28" t="s">
+      <c r="T28" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>66</v>
       </c>
@@ -2374,31 +2551,37 @@
         <v>160</v>
       </c>
       <c r="K29" t="s">
+        <v>236</v>
+      </c>
+      <c r="L29" t="s">
         <v>40</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>21</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>48</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>43</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q29" t="s">
         <v>108</v>
       </c>
-      <c r="P29" t="s">
+      <c r="R29" t="s">
         <v>145</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="S29" t="s">
         <v>146</v>
       </c>
-      <c r="R29" t="s">
+      <c r="T29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>71</v>
       </c>
@@ -2421,31 +2604,37 @@
         <v>162</v>
       </c>
       <c r="K30" t="s">
+        <v>236</v>
+      </c>
+      <c r="L30" t="s">
         <v>40</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>21</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>48</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>43</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q30" t="s">
         <v>86</v>
       </c>
-      <c r="P30" t="s">
+      <c r="R30" t="s">
         <v>63</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="S30" t="s">
         <v>64</v>
       </c>
-      <c r="R30" t="s">
+      <c r="T30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>79</v>
       </c>
@@ -2468,31 +2657,37 @@
         <v>164</v>
       </c>
       <c r="K31" t="s">
+        <v>236</v>
+      </c>
+      <c r="L31" t="s">
         <v>108</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>145</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>146</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>111</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q31" t="s">
         <v>165</v>
       </c>
-      <c r="P31" t="s">
+      <c r="R31" t="s">
         <v>21</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="S31" t="s">
         <v>116</v>
       </c>
-      <c r="R31" t="s">
+      <c r="T31" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>80</v>
       </c>
@@ -2515,31 +2710,37 @@
         <v>168</v>
       </c>
       <c r="K32" t="s">
+        <v>236</v>
+      </c>
+      <c r="L32" t="s">
         <v>108</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>145</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>146</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>111</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q32" t="s">
         <v>115</v>
       </c>
-      <c r="P32" t="s">
+      <c r="R32" t="s">
         <v>21</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="S32" t="s">
         <v>116</v>
       </c>
-      <c r="R32" t="s">
+      <c r="T32" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>81</v>
       </c>
@@ -2556,31 +2757,37 @@
         <v>170</v>
       </c>
       <c r="K33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L33" t="s">
         <v>108</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>121</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>103</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>111</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q33" t="s">
         <v>101</v>
       </c>
-      <c r="P33" t="s">
+      <c r="R33" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="S33" t="s">
         <v>48</v>
       </c>
-      <c r="R33" t="s">
+      <c r="T33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>82</v>
       </c>
@@ -2597,31 +2804,37 @@
         <v>172</v>
       </c>
       <c r="K34" t="s">
+        <v>236</v>
+      </c>
+      <c r="L34" t="s">
         <v>108</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>145</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>146</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>111</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q34" t="s">
         <v>86</v>
       </c>
-      <c r="P34" t="s">
+      <c r="R34" t="s">
         <v>37</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="S34" t="s">
         <v>87</v>
       </c>
-      <c r="R34" t="s">
+      <c r="T34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>89</v>
       </c>
@@ -2638,31 +2851,37 @@
         <v>174</v>
       </c>
       <c r="K35" t="s">
+        <v>236</v>
+      </c>
+      <c r="L35" t="s">
         <v>175</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>176</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>177</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>178</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q35" t="s">
         <v>175</v>
       </c>
-      <c r="P35" t="s">
+      <c r="R35" t="s">
         <v>176</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="S35" t="s">
         <v>177</v>
       </c>
-      <c r="R35" t="s">
+      <c r="T35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>90</v>
       </c>
@@ -2679,31 +2898,37 @@
         <v>180</v>
       </c>
       <c r="K36" t="s">
+        <v>236</v>
+      </c>
+      <c r="L36" t="s">
         <v>157</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>74</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>26</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>158</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q36" t="s">
         <v>59</v>
       </c>
-      <c r="P36" t="s">
+      <c r="R36" t="s">
         <v>63</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="S36" t="s">
         <v>64</v>
       </c>
-      <c r="R36" t="s">
+      <c r="T36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>92</v>
       </c>
@@ -2720,27 +2945,33 @@
         <v>182</v>
       </c>
       <c r="K37" t="s">
+        <v>236</v>
+      </c>
+      <c r="L37" t="s">
         <v>59</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>60</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>61</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>62</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q37" t="s">
         <v>59</v>
       </c>
-      <c r="P37" t="s">
+      <c r="R37" t="s">
         <v>60</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="S37" t="s">
         <v>61</v>
       </c>
-      <c r="R37" t="s">
+      <c r="T37" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>